<commit_message>
resetting restriction: admin can only delete data from last academic year
</commit_message>
<xml_diff>
--- a/static/file/student_example.xlsx
+++ b/static/file/student_example.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>chinese_name</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>user_name</t>
+  </si>
+  <si>
+    <t>graduation_year</t>
   </si>
   <si>
     <t>学生一</t>
@@ -84,7 +87,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +107,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -570,146 +566,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1067,13 +1063,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.1666666666667" customWidth="1"/>
     <col min="2" max="2" width="20.3333333333333" customWidth="1"/>
@@ -1083,7 +1079,7 @@
     <col min="6" max="6" width="19.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,39 +1095,48 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>